<commit_message>
updates syllabus to push back homework reflection 4 by one week
</commit_message>
<xml_diff>
--- a/syllabus/438-syllabus.xlsx
+++ b/syllabus/438-syllabus.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="20910"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="24526"/>
   <workbookPr date1904="1" showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="14980" tabRatio="500"/>
@@ -303,12 +303,6 @@
     <t>Reflection 3</t>
   </si>
   <si>
-    <t>Reflection 4</t>
-  </si>
-  <si>
-    <t>Reflection 5</t>
-  </si>
-  <si>
     <t>REEPS 9.1 - 9.4</t>
   </si>
   <si>
@@ -319,6 +313,12 @@
   </si>
   <si>
     <t>REEPS 8.5 - 8.8</t>
+  </si>
+  <si>
+    <t>Homework Reflection 4</t>
+  </si>
+  <si>
+    <t>Homework Reflection 5</t>
   </si>
 </sst>
 </file>
@@ -331,7 +331,6 @@
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
-      <charset val="238"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -420,8 +419,10 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="35">
+  <cellStyleXfs count="37">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -483,7 +484,7 @@
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
-  <cellStyles count="35">
+  <cellStyles count="37">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -501,6 +502,7 @@
     <cellStyle name="Followed Hyperlink" xfId="30" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="32" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="34" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="36" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -518,6 +520,7 @@
     <cellStyle name="Hyperlink" xfId="29" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="31" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="33" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="35" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -853,7 +856,7 @@
   <dimension ref="A1:I32"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="D24" sqref="D24"/>
+      <selection activeCell="F33" sqref="F33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -863,7 +866,7 @@
     <col min="3" max="3" width="9.83203125" style="1" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="35.1640625" style="1" customWidth="1"/>
     <col min="5" max="5" width="12.5" style="1" customWidth="1"/>
-    <col min="6" max="6" width="10.83203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="20.33203125" style="1" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="16.83203125" style="1" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="5" style="1" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="16" style="1" bestFit="1" customWidth="1"/>
@@ -1404,7 +1407,7 @@
       <c r="G24" s="4"/>
       <c r="H24" s="4"/>
       <c r="I24" s="4" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
     </row>
     <row r="25" spans="1:9" s="5" customFormat="1" ht="18" customHeight="1">
@@ -1431,7 +1434,7 @@
       </c>
       <c r="H25" s="4"/>
       <c r="I25" s="4" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
     </row>
     <row r="26" spans="1:9" s="5" customFormat="1" ht="18" customHeight="1">
@@ -1454,7 +1457,7 @@
       <c r="G26" s="4"/>
       <c r="H26" s="4"/>
       <c r="I26" s="4" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
     </row>
     <row r="27" spans="1:9" s="5" customFormat="1" ht="18" customHeight="1">
@@ -1481,7 +1484,7 @@
       </c>
       <c r="H27" s="4"/>
       <c r="I27" s="4" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
     </row>
     <row r="28" spans="1:9" s="5" customFormat="1" ht="18" customHeight="1">
@@ -1519,9 +1522,6 @@
         <v>79</v>
       </c>
       <c r="E29" s="4"/>
-      <c r="F29" s="4" t="s">
-        <v>94</v>
-      </c>
       <c r="G29" s="4"/>
       <c r="H29" s="4"/>
       <c r="I29" s="4"/>
@@ -1561,7 +1561,9 @@
         <v>38</v>
       </c>
       <c r="E31" s="4"/>
-      <c r="F31" s="4"/>
+      <c r="F31" s="4" t="s">
+        <v>98</v>
+      </c>
       <c r="G31" s="4"/>
       <c r="H31" s="4"/>
       <c r="I31" s="4"/>
@@ -1581,7 +1583,7 @@
       </c>
       <c r="E32" s="4"/>
       <c r="F32" s="4" t="s">
-        <v>95</v>
+        <v>99</v>
       </c>
       <c r="G32" s="4"/>
       <c r="H32" s="4"/>

</xml_diff>